<commit_message>
added NB classifier from scratch
</commit_message>
<xml_diff>
--- a/5. Text Mining/Naive_Bayes_from_scratch.xlsx
+++ b/5. Text Mining/Naive_Bayes_from_scratch.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10503"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paragpradhan/Documents/Data Science Course/DS-Intro/8.Text_Mining/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paragpradhan/Documents/Data Science Course/DSB4/5. Text Mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81334DAF-567D-A044-A82D-D980E77F6DD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ADAE93-A4E1-8246-B9FA-A315C600E59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16000" windowHeight="10720" xr2:uid="{EA76C76F-82A6-2E4D-914E-96F3EB9CCF2A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EA76C76F-82A6-2E4D-914E-96F3EB9CCF2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Exercise" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
   <si>
     <t>Hi you have won lottery</t>
   </si>
@@ -149,6 +151,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>meeting at management cabin</t>
+  </si>
+  <si>
+    <t>P(meeting | spam)</t>
+  </si>
+  <si>
+    <t>P(at| spam)</t>
+  </si>
+  <si>
+    <t>P(management | spam)</t>
+  </si>
+  <si>
+    <t>P(cabin | spam)</t>
+  </si>
+  <si>
+    <t>P(meeting | ham)</t>
+  </si>
+  <si>
+    <t>P(at| ham)</t>
+  </si>
+  <si>
+    <t>P(management | ham)</t>
+  </si>
+  <si>
+    <t>P(cabin | ham)</t>
   </si>
 </sst>
 </file>
@@ -159,7 +188,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -563,9 +592,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -573,7 +602,7 @@
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -581,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1">
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -598,7 +627,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" thickTop="1">
+    <row r="3" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -613,7 +642,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -621,7 +650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -629,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -640,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -648,7 +677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -656,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -667,7 +696,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -675,7 +704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -692,7 +721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -714,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -722,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" ref="C15:C18" si="0">B15/$B$8</f>
+        <f t="shared" ref="C15:C17" si="0">B15/$B$8</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="D15" t="s">
@@ -732,11 +761,11 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F18" si="1">E15/$B$9</f>
+        <f t="shared" ref="F15:F17" si="1">E15/$B$9</f>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -758,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -780,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -802,7 +831,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" s="9">
         <f>C14*C15*C16*C17*C18</f>
         <v>0</v>
@@ -814,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -822,7 +851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" thickBot="1">
+    <row r="22" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -830,13 +859,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
@@ -853,7 +882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -875,7 +904,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -897,7 +926,7 @@
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -919,7 +948,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -941,7 +970,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
@@ -963,7 +992,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6">
@@ -985,13 +1014,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD162F87-0472-3E4A-9878-3941F076504F}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -999,7 +1028,7 @@
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1007,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1">
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1050,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" thickTop="1">
+    <row r="3" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1033,7 +1062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1049,20 +1078,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1070,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1078,7 +1107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1086,272 +1115,216 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
-        <f>0/7</f>
-        <v>0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F14">
         <f>E14/$B$9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8">
-        <f xml:space="preserve"> 1 / 7</f>
-        <v>0.14285714285714285</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C15" s="8"/>
       <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E15" s="3"/>
       <c r="F15">
         <f t="shared" ref="F15:F17" si="0">E15/$B$9</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7">
-        <f>1/7</f>
-        <v>0.14285714285714285</v>
-      </c>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>29</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7">
-        <f>2/7</f>
-        <v>0.2857142857142857</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="7">
         <f>2/5</f>
         <v>0.4</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <f>3/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" thickBot="1">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <f>(B26+1)/($B$8 + $B$10)</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <f>(E26+1)/($B$9 + $B$10)</f>
-        <v>3.2258064516129031E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <f t="shared" ref="C27:C29" si="1">(B27+1)/($B$8 + $B$10)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C27" s="7"/>
       <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <f t="shared" ref="F27:F29" si="2">(E27+1)/($B$9 + $B$10)</f>
-        <v>6.4516129032258063E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" s="7"/>
+      <c r="D29" t="s">
         <v>29</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>3.2258064516129031E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="2"/>
-        <v>3.2258064516129031E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="9">
+      <c r="B32" s="6"/>
+      <c r="C32" s="9">
         <f>2/5</f>
         <v>0.4</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6">
+      <c r="E32" s="6"/>
+      <c r="F32" s="6">
         <f>3/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6">
-        <f>C26*C27*C28*C29*C30</f>
-        <v>1.4467592592592593E-5</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6">
-        <f>F26*F27*F28*F29*F30</f>
-        <v>1.2993748923955163E-6</v>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6">
+        <f>C27*C28*C29*C30*C32</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6">
+        <f>F27*F28*F29*F30*F32</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>